<commit_message>
planned out teh ap
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>TO DO LIST</t>
   </si>
@@ -61,13 +61,88 @@
   </si>
   <si>
     <t>delete task</t>
+  </si>
+  <si>
+    <t>toggle button</t>
+  </si>
+  <si>
+    <t>the toggle button so you can see all weeks or just this week.</t>
+  </si>
+  <si>
+    <t>to do list</t>
+  </si>
+  <si>
+    <t>Task:</t>
+  </si>
+  <si>
+    <t>Paint the guest room's ensuite's wall peach</t>
+  </si>
+  <si>
+    <t>Due Date:</t>
+  </si>
+  <si>
+    <t>have this as a wheely calandar</t>
+  </si>
+  <si>
+    <t>A drop down box of maybe 3 colours marked HIGH, MEDIUM, LOW</t>
+  </si>
+  <si>
+    <t>INPUT SECTION</t>
+  </si>
+  <si>
+    <t>Priority Colour:</t>
+  </si>
+  <si>
+    <t>Current to-do list</t>
+  </si>
+  <si>
+    <t>need the TASK to squish down onto a number of lines as screen size varies</t>
+  </si>
+  <si>
+    <t>Buy peach paint</t>
+  </si>
+  <si>
+    <t>Buy Bananas</t>
+  </si>
+  <si>
+    <t>if sorting by date how does comp know what order?</t>
+  </si>
+  <si>
+    <t>Buy Alan a beer</t>
+  </si>
+  <si>
+    <t>Completed to do list</t>
+  </si>
+  <si>
+    <t>DONE BUTTON</t>
+  </si>
+  <si>
+    <t>Drink a rum and coke</t>
+  </si>
+  <si>
+    <t>Make a gin and lemonade</t>
+  </si>
+  <si>
+    <t>Watch season 9 of Curb your enthiasm</t>
+  </si>
+  <si>
+    <t>hover over DELETE BUTTON</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Add back to TO DO LIST BUTTON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +150,77 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -167,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -175,6 +314,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,35 +658,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="15" style="23" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,33 +704,33 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -546,14 +738,14 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -561,12 +753,12 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -574,12 +766,12 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -587,23 +779,23 @@
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -614,9 +806,183 @@
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="11">
+        <v>43952</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="E26" s="26">
+        <v>43946</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="19"/>
+      <c r="E27" s="27">
+        <v>43946</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="19"/>
+      <c r="E28" s="28">
+        <v>43952</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="21"/>
+      <c r="E29" s="29">
+        <v>43983</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="18"/>
+      <c r="C32" s="17"/>
+      <c r="E32" s="31">
+        <v>43944</v>
+      </c>
+      <c r="F32" s="31">
+        <v>43945</v>
+      </c>
+      <c r="G32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="17"/>
+      <c r="E33" s="31">
+        <v>43944</v>
+      </c>
+      <c r="F33" s="31">
+        <v>43944</v>
+      </c>
+      <c r="G33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="17"/>
+      <c r="E34" s="31">
+        <v>43940</v>
+      </c>
+      <c r="F34" s="31">
+        <v>43938</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added a new toggle option
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>TO DO LIST</t>
   </si>
@@ -136,13 +136,28 @@
   </si>
   <si>
     <t>Add back to TO DO LIST BUTTON</t>
+  </si>
+  <si>
+    <t>OPTION TOGGLED TO ALL WEEKS</t>
+  </si>
+  <si>
+    <t>NEXT WEEK</t>
+  </si>
+  <si>
+    <t>THIS WEEK</t>
+  </si>
+  <si>
+    <t>W/C 01/06/2020</t>
+  </si>
+  <si>
+    <t>OPTION TOGGLED TO THIS WEEK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +205,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -223,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -302,11 +326,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -314,21 +418,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -339,24 +437,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,8 +806,8 @@
     <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="15" style="23" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15" style="17" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
@@ -682,19 +818,19 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -704,18 +840,18 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -738,7 +874,7 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -753,7 +889,7 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="5"/>
@@ -766,7 +902,7 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="5"/>
@@ -779,7 +915,7 @@
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="6"/>
@@ -809,180 +945,788 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="24"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="27"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="27"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="27"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="12">
         <v>43952</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="27"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="27"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="27"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="27"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="27"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="E26" s="26">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="32">
         <v>43946</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F27" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H27" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="27"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="19"/>
-      <c r="E27" s="27">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="20">
         <v>43946</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F28" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H28" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="27"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="27"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="19"/>
-      <c r="E28" s="28">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="20">
         <v>43952</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F30" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="27"/>
+    </row>
+    <row r="31" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="50"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="21"/>
-      <c r="E29" s="29">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="35">
         <v>43983</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F32" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G32" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="27"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="27"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F34" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G34" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="27"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="17"/>
-      <c r="E32" s="31">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="38">
         <v>43944</v>
       </c>
-      <c r="F32" s="31">
+      <c r="F35" s="38">
         <v>43945</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G35" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="27"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="17"/>
-      <c r="E33" s="31">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="38">
         <v>43944</v>
       </c>
-      <c r="F33" s="31">
+      <c r="F36" s="38">
         <v>43944</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G36" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="27"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="17"/>
-      <c r="E34" s="31">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="38">
         <v>43940</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F37" s="38">
         <v>43938</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G37" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="27"/>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="39"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="42"/>
+    </row>
+    <row r="39" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="24"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="27"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="27"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="27"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="12">
+        <v>43952</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="27"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="27"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="29"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="27"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="27"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="27"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="32">
+        <v>43946</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="27"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="20">
+        <v>43946</v>
+      </c>
+      <c r="F50" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="27"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="29"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="27"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F52" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="27"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="38">
+        <v>43944</v>
+      </c>
+      <c r="F53" s="38">
+        <v>43945</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="27"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="38">
+        <v>43944</v>
+      </c>
+      <c r="F54" s="38">
+        <v>43944</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="27"/>
+    </row>
+    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="39"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+      <c r="O55" s="42"/>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>